<commit_message>
Diagnostic Report FHIR IG - completed Simple Pathology Observation
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/observation-path-simple-1.xlsx
+++ b/output/DiagnosticReport/observation-path-simple-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="468">
   <si>
     <t>Path</t>
   </si>
@@ -166,7 +166,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}obs-7:If Observation.code is the same as an Observation.component.code then the value element associated with the code SHALL NOT be present {value.empty() or component.code.where(coding.intersect(%resource.code.coding).exists()).empty()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}obs-7:If Observation.code is the same as an Observation.component.code then the value element associated with the code SHALL NOT be present {value.empty() or component.code.where(coding.intersect(%resource.code.coding).exists()).empty()}inv-dh-obs-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -481,7 +481,7 @@
     <t>Observation.status</t>
   </si>
   <si>
-    <t>registered | preliminary | final | amended +</t>
+    <t>preliminary | final | amended +</t>
   </si>
   <si>
     <t>The status of the result value.</t>
@@ -496,10 +496,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>Codes providing the status of an observation.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-status|4.0.1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/observationstatus-result-available-1</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -575,13 +572,7 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/pathology-procedure-1</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -700,7 +691,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>
@@ -1010,6 +1001,9 @@
   <si>
     <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   
 If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ bodySite](http://hl7.org/fhir/R4/extension-bodysite.html).</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1449,6 +1443,12 @@
   </si>
   <si>
     <t>*All* code-value and  component.code-component.value pairs need to be taken into account to correctly understand the meaning of the observation.</t>
+  </si>
+  <si>
+    <t>Codes identifying names of simple observations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>&lt; 363787002 |Observable entity| OR @@ -1671,7 +1671,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="64.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="78.2890625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -3396,11 +3396,9 @@
       <c r="W15" t="s" s="2">
         <v>151</v>
       </c>
-      <c r="X15" t="s" s="2">
+      <c r="X15" s="2"/>
+      <c r="Y15" t="s" s="2">
         <v>152</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>153</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3433,19 +3431,19 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="AK15" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="AK15" t="s" s="2">
+      <c r="AL15" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="AL15" t="s" s="2">
+      <c r="AM15" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="AM15" t="s" s="2">
+      <c r="AN15" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="AN15" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3453,7 +3451,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3476,19 +3474,19 @@
         <v>45</v>
       </c>
       <c r="J16" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="K16" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="K16" t="s" s="2">
+      <c r="L16" t="s" s="2">
         <v>161</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="M16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>163</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>164</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3498,7 +3496,7 @@
         <v>45</v>
       </c>
       <c r="R16" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S16" t="s" s="2">
         <v>45</v>
@@ -3516,11 +3514,11 @@
         <v>79</v>
       </c>
       <c r="X16" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="Y16" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="Y16" t="s" s="2">
-        <v>167</v>
-      </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
       </c>
@@ -3537,7 +3535,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>43</v>
@@ -3561,10 +3559,10 @@
         <v>45</v>
       </c>
       <c r="AM16" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="AN16" t="s" s="2">
         <v>168</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>169</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3572,11 +3570,11 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3595,19 +3593,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K17" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>174</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>175</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3632,13 +3630,11 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="X17" t="s" s="2">
-        <v>177</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="X17" s="2"/>
       <c r="Y17" t="s" s="2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3656,7 +3652,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>55</v>
@@ -3671,27 +3667,27 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AO17" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="AO17" t="s" s="2">
-        <v>184</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3717,10 +3713,10 @@
         <v>57</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3771,7 +3767,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3795,7 +3791,7 @@
         <v>45</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>45</v>
@@ -3806,7 +3802,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3832,10 +3828,10 @@
         <v>100</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M19" t="s" s="2">
         <v>116</v>
@@ -3879,7 +3875,7 @@
         <v>103</v>
       </c>
       <c r="AB19" t="s" s="2">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AC19" t="s" s="2">
         <v>45</v>
@@ -3888,7 +3884,7 @@
         <v>104</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3912,7 +3908,7 @@
         <v>45</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>45</v>
@@ -3923,7 +3919,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3946,19 +3942,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="M20" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3995,7 +3991,7 @@
         <v>45</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AB20" s="2"/>
       <c r="AC20" t="s" s="2">
@@ -4005,7 +4001,7 @@
         <v>104</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -4026,10 +4022,10 @@
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>45</v>
@@ -4040,10 +4036,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>45</v>
@@ -4065,19 +4061,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="K21" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>199</v>
-      </c>
       <c r="N21" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -4106,7 +4102,7 @@
       </c>
       <c r="X21" s="2"/>
       <c r="Y21" t="s" s="2">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>45</v>
@@ -4124,7 +4120,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -4145,10 +4141,10 @@
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>45</v>
@@ -4159,7 +4155,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4185,16 +4181,16 @@
         <v>57</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="N22" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4243,7 +4239,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4264,10 +4260,10 @@
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>45</v>
@@ -4278,7 +4274,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4301,19 +4297,19 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="M23" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4362,7 +4358,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4377,19 +4373,19 @@
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AK23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AM23" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AN23" t="s" s="2">
         <v>222</v>
-      </c>
-      <c r="AK23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL23" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AM23" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>225</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4397,7 +4393,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4420,16 +4416,16 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="M24" t="s" s="2">
         <v>227</v>
-      </c>
-      <c r="K24" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>230</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -4479,7 +4475,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4500,13 +4496,13 @@
         <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4514,11 +4510,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4537,19 +4533,19 @@
         <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="K25" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="L25" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="M25" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="N25" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4598,7 +4594,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4613,19 +4609,19 @@
         <v>67</v>
       </c>
       <c r="AJ25" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="AK25" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="AM25" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AN25" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="AK25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL25" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="AM25" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>242</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>45</v>
@@ -4633,11 +4629,11 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4656,19 +4652,19 @@
         <v>56</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="M26" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>249</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4717,7 +4713,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4732,19 +4728,19 @@
         <v>67</v>
       </c>
       <c r="AJ26" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="AK26" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL26" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AM26" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="AN26" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="AK26" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL26" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="AM26" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="AN26" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>45</v>
@@ -4752,7 +4748,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4775,16 +4771,16 @@
         <v>56</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="K27" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="K27" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4834,7 +4830,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4855,13 +4851,13 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>45</v>
@@ -4869,7 +4865,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4892,17 +4888,17 @@
         <v>56</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" t="s" s="2">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4951,7 +4947,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4966,19 +4962,19 @@
         <v>67</v>
       </c>
       <c r="AJ28" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="AK28" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL28" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="AM28" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AN28" t="s" s="2">
         <v>267</v>
-      </c>
-      <c r="AK28" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL28" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AN28" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>45</v>
@@ -4986,7 +4982,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5009,19 +5005,19 @@
         <v>56</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="M29" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>276</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
@@ -5070,7 +5066,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -5079,7 +5075,7 @@
         <v>55</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>67</v>
@@ -5088,24 +5084,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AM29" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>278</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="AM29" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>281</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5128,19 +5124,19 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="N30" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -5165,13 +5161,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -5189,7 +5185,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5198,7 +5194,7 @@
         <v>55</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>67</v>
@@ -5213,7 +5209,7 @@
         <v>98</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5224,11 +5220,11 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -5247,19 +5243,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="N31" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5284,13 +5280,13 @@
         <v>45</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>45</v>
@@ -5308,7 +5304,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5326,24 +5322,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AL31" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AM31" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AN31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO31" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AN31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO31" t="s" s="2">
-        <v>303</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5366,19 +5362,19 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="K32" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L32" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="M32" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
@@ -5427,7 +5423,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5448,10 +5444,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5462,7 +5458,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5485,16 +5481,16 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
@@ -5520,13 +5516,13 @@
         <v>45</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>176</v>
+        <v>313</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>45</v>
@@ -5544,7 +5540,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5562,24 +5558,24 @@
         <v>45</v>
       </c>
       <c r="AK33" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AL33" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AM33" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="AL33" t="s" s="2">
+      <c r="AN33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO33" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="AM33" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="AN33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO33" t="s" s="2">
-        <v>321</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5602,19 +5598,19 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="M34" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="N34" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5639,13 +5635,13 @@
         <v>45</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>176</v>
+        <v>313</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>45</v>
@@ -5663,7 +5659,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5684,10 +5680,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5698,7 +5694,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5721,16 +5717,16 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>332</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -5780,7 +5776,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5798,24 +5794,24 @@
         <v>45</v>
       </c>
       <c r="AK35" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="AL35" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="AL35" t="s" s="2">
+      <c r="AN35" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO35" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="AN35" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO35" t="s" s="2">
-        <v>339</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5838,16 +5834,16 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="K36" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>341</v>
       </c>
-      <c r="K36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5897,7 +5893,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5915,24 +5911,24 @@
         <v>45</v>
       </c>
       <c r="AK36" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AL36" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="AM36" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO36" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="AM36" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="AN36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO36" t="s" s="2">
-        <v>348</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5955,19 +5951,19 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="K37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>352</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -6016,7 +6012,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -6028,19 +6024,19 @@
         <v>45</v>
       </c>
       <c r="AI37" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL37" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="AM37" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="AJ37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="AM37" t="s" s="2">
-        <v>357</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -6051,7 +6047,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6077,10 +6073,10 @@
         <v>57</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -6131,7 +6127,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6155,7 +6151,7 @@
         <v>45</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6166,7 +6162,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6192,10 +6188,10 @@
         <v>100</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M39" t="s" s="2">
         <v>116</v>
@@ -6248,7 +6244,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6272,7 +6268,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6283,11 +6279,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -6309,10 +6305,10 @@
         <v>100</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M40" t="s" s="2">
         <v>116</v>
@@ -6367,7 +6363,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6402,7 +6398,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6425,13 +6421,13 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="K41" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>368</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6482,7 +6478,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6491,7 +6487,7 @@
         <v>55</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>67</v>
@@ -6503,10 +6499,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6517,7 +6513,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6540,13 +6536,13 @@
         <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6597,7 +6593,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6606,7 +6602,7 @@
         <v>55</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>67</v>
@@ -6618,10 +6614,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6632,7 +6628,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6655,19 +6651,19 @@
         <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>380</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6695,10 +6691,10 @@
         <v>79</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6716,7 +6712,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6734,13 +6730,13 @@
         <v>45</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6751,7 +6747,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6774,19 +6770,19 @@
         <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>389</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -6811,13 +6807,13 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>176</v>
+        <v>313</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
@@ -6835,7 +6831,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6853,13 +6849,13 @@
         <v>45</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6870,7 +6866,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6893,17 +6889,17 @@
         <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="K45" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -6952,7 +6948,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6976,7 +6972,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6987,7 +6983,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7013,10 +7009,10 @@
         <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -7067,7 +7063,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7088,10 +7084,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -7102,7 +7098,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7125,16 +7121,16 @@
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="K47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -7184,7 +7180,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7205,10 +7201,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7219,7 +7215,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7245,10 +7241,10 @@
         <v>57</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -7299,7 +7295,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7323,7 +7319,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7334,7 +7330,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7360,10 +7356,10 @@
         <v>100</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M49" t="s" s="2">
         <v>116</v>
@@ -7407,7 +7403,7 @@
         <v>103</v>
       </c>
       <c r="AB49" t="s" s="2">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AC49" t="s" s="2">
         <v>45</v>
@@ -7416,7 +7412,7 @@
         <v>104</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7440,7 +7436,7 @@
         <v>45</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7451,7 +7447,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7477,13 +7473,13 @@
         <v>57</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7533,7 +7529,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7542,7 +7538,7 @@
         <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>67</v>
@@ -7568,7 +7564,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7594,13 +7590,13 @@
         <v>69</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>418</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7626,31 +7622,31 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="X51" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE51" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7685,7 +7681,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7711,13 +7707,13 @@
         <v>120</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>427</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7767,7 +7763,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7791,7 +7787,7 @@
         <v>45</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7802,7 +7798,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7828,13 +7824,13 @@
         <v>57</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
@@ -7884,7 +7880,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7919,7 +7915,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7942,16 +7938,16 @@
         <v>56</v>
       </c>
       <c r="J54" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>436</v>
       </c>
-      <c r="K54" t="s" s="2">
+      <c r="M54" t="s" s="2">
         <v>437</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>439</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
@@ -8001,7 +7997,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8022,10 +8018,10 @@
         <v>45</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8036,7 +8032,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8059,19 +8055,19 @@
         <v>56</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="N55" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>445</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>45</v>
@@ -8120,7 +8116,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8141,10 +8137,10 @@
         <v>45</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8155,7 +8151,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8181,10 +8177,10 @@
         <v>57</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -8235,7 +8231,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8259,7 +8255,7 @@
         <v>45</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
@@ -8270,7 +8266,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8296,10 +8292,10 @@
         <v>100</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M57" t="s" s="2">
         <v>116</v>
@@ -8352,7 +8348,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8376,7 +8372,7 @@
         <v>45</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
@@ -8387,11 +8383,11 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8413,10 +8409,10 @@
         <v>100</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M58" t="s" s="2">
         <v>116</v>
@@ -8471,7 +8467,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8506,7 +8502,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8529,19 +8525,19 @@
         <v>56</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="L59" t="s" s="2">
-        <v>453</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>454</v>
-      </c>
       <c r="N59" t="s" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8566,13 +8562,13 @@
         <v>45</v>
       </c>
       <c r="W59" t="s" s="2">
-        <v>176</v>
+        <v>313</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>177</v>
+        <v>453</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>178</v>
+        <v>454</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>45</v>
@@ -8590,7 +8586,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>55</v>
@@ -8611,13 +8607,13 @@
         <v>455</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AO59" t="s" s="2">
         <v>45</v>
@@ -8648,19 +8644,19 @@
         <v>56</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="K60" t="s" s="2">
         <v>457</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>458</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>45</v>
@@ -8730,16 +8726,16 @@
         <v>459</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" hidden="true">
@@ -8767,7 +8763,7 @@
         <v>45</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K61" t="s" s="2">
         <v>461</v>
@@ -8779,7 +8775,7 @@
         <v>463</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -8804,13 +8800,13 @@
         <v>45</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>45</v>
@@ -8837,7 +8833,7 @@
         <v>55</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>67</v>
@@ -8852,7 +8848,7 @@
         <v>98</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -8867,7 +8863,7 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
@@ -8886,19 +8882,19 @@
         <v>45</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="N62" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
@@ -8923,13 +8919,13 @@
         <v>45</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>45</v>
@@ -8965,19 +8961,19 @@
         <v>45</v>
       </c>
       <c r="AK62" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AM62" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AN62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO62" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="AM62" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO62" t="s" s="2">
-        <v>303</v>
       </c>
     </row>
     <row r="63" hidden="true">
@@ -9014,10 +9010,10 @@
         <v>467</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>45</v>
@@ -9087,10 +9083,10 @@
         <v>45</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>45</v>

</xml_diff>